<commit_message>
Se actualiza cronograma despues de reunion del domingo
</commit_message>
<xml_diff>
--- a/Cronograma proyecto fundamentos SW.xlsx
+++ b/Cronograma proyecto fundamentos SW.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\Proyecto_Discoteca\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE48436-F228-46ED-8066-E547744858E0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B964F7-E512-477D-8D64-E75A8C45B2CD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{D986376F-8C97-4DB8-A64D-C8306675A2D3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="57">
   <si>
     <t>Cronograma de iteraciones</t>
   </si>
@@ -134,9 +134,6 @@
     <t>Crear MVC Front End</t>
   </si>
   <si>
-    <t>Crear MVC Base de datos</t>
-  </si>
-  <si>
     <t>Crear MVC de control</t>
   </si>
   <si>
@@ -161,9 +158,6 @@
     <t>*</t>
   </si>
   <si>
-    <t>Crear flujo normal Caso de Uso 1</t>
-  </si>
-  <si>
     <t>Crear pantalla de primer Casos de Uso</t>
   </si>
   <si>
@@ -173,9 +167,6 @@
     <t>Revisión de errores de código</t>
   </si>
   <si>
-    <t>corrección de pantallas</t>
-  </si>
-  <si>
     <t>corrección de errores de código</t>
   </si>
   <si>
@@ -185,9 +176,6 @@
     <t>Documentación de Caso de Uso 1</t>
   </si>
   <si>
-    <t>Oracle SQL preferiblemente. Suficiente: SQL Lite</t>
-  </si>
-  <si>
     <t>Revisar modelo relacional</t>
   </si>
   <si>
@@ -210,6 +198,15 @@
   </si>
   <si>
     <t>Columna1</t>
+  </si>
+  <si>
+    <t>Todos</t>
+  </si>
+  <si>
+    <t>Corrección de pantallas</t>
+  </si>
+  <si>
+    <t>Revisar avances y ajustar cronograma</t>
   </si>
 </sst>
 </file>
@@ -403,8 +400,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A72A92D3-E334-4DD1-8B5B-9E136970B0F3}" name="Tabla3" displayName="Tabla3" ref="A3:H49" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A3:H49" xr:uid="{9BEBBDC5-EE9F-4F4A-BDEB-F8F8B36213DC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A72A92D3-E334-4DD1-8B5B-9E136970B0F3}" name="Tabla3" displayName="Tabla3" ref="A3:H46" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A3:H46" xr:uid="{9BEBBDC5-EE9F-4F4A-BDEB-F8F8B36213DC}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{45061F07-E9EB-42CA-BAE5-F676D0C08594}" name="Iteracion"/>
     <tableColumn id="2" xr3:uid="{74201B4C-A788-4118-B00F-B1DF78D97842}" name="Semana iteración"/>
@@ -716,12 +713,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{676346D6-29B9-4D30-B57C-A0159E888A1C}">
-  <dimension ref="A2:H49"/>
+  <dimension ref="A2:H46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
+      <selection pane="bottomLeft" activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,7 +768,7 @@
         <v>5</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -977,50 +974,60 @@
       <c r="D12" s="1">
         <v>44974</v>
       </c>
+      <c r="E12" s="1">
+        <v>44973</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>19</v>
+      </c>
       <c r="G12" s="8">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13">
+      <c r="A13" s="13">
+        <v>1</v>
+      </c>
+      <c r="B13" s="13">
         <v>2</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="14" t="s">
         <v>33</v>
       </c>
       <c r="D13" s="1">
-        <v>44974</v>
+        <v>44975</v>
       </c>
       <c r="E13" s="1">
-        <v>44973</v>
+        <v>44975</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="8">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="G13" s="16">
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="13">
-        <v>1</v>
-      </c>
-      <c r="B14" s="13">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
         <v>2</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D14" s="1">
         <v>44975</v>
       </c>
-      <c r="E14" s="15"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="16">
-        <v>20</v>
+      <c r="E14" s="1">
+        <v>44975</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="8">
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1034,10 +1041,16 @@
         <v>35</v>
       </c>
       <c r="D15" s="1">
+        <v>44976</v>
+      </c>
+      <c r="E15" s="1">
         <v>44975</v>
       </c>
+      <c r="F15" s="14" t="s">
+        <v>27</v>
+      </c>
       <c r="G15" s="8">
-        <v>30</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1053,6 +1066,12 @@
       <c r="D16" s="1">
         <v>44976</v>
       </c>
+      <c r="E16" s="1">
+        <v>44975</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="G16" s="8">
         <v>60</v>
       </c>
@@ -1070,8 +1089,17 @@
       <c r="D17" s="1">
         <v>44976</v>
       </c>
+      <c r="E17" s="1">
+        <v>44976</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="G17" s="8">
         <v>60</v>
+      </c>
+      <c r="H17" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1082,16 +1110,19 @@
         <v>2</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="D18" s="1">
         <v>44976</v>
       </c>
+      <c r="E18" s="1">
+        <v>44974</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="G18" s="8">
-        <v>60</v>
-      </c>
-      <c r="H18" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1102,10 +1133,10 @@
         <v>2</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="D19" s="1">
-        <v>44976</v>
+        <v>44977</v>
       </c>
       <c r="E19" s="1">
         <v>44974</v>
@@ -1114,7 +1145,7 @@
         <v>19</v>
       </c>
       <c r="G19" s="8">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1130,74 +1161,74 @@
       <c r="D20" s="1">
         <v>44977</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>40</v>
+      <c r="E20" s="1">
+        <v>44976</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="G20" s="8">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>1</v>
-      </c>
-      <c r="B21">
+      <c r="A21" s="9">
+        <v>1</v>
+      </c>
+      <c r="B21" s="9">
         <v>2</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" s="1">
-        <v>44977</v>
-      </c>
-      <c r="E21" s="1">
-        <v>44974</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G21" s="8">
-        <v>60</v>
-      </c>
+      <c r="C21" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="11">
+        <v>44979</v>
+      </c>
+      <c r="E21" s="11"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="12">
+        <v>60</v>
+      </c>
+      <c r="H21" s="9"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>1</v>
-      </c>
-      <c r="B22">
+      <c r="A22" s="9">
+        <v>1</v>
+      </c>
+      <c r="B22" s="9">
         <v>2</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="1">
-        <v>44977</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G22" s="8">
-        <v>20</v>
-      </c>
+      <c r="C22" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="11">
+        <v>44979</v>
+      </c>
+      <c r="E22" s="11"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="12">
+        <v>60</v>
+      </c>
+      <c r="H22" s="9"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
       <c r="B23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="D23" s="1">
-        <v>44977</v>
+        <v>45009</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G23" s="8">
-        <v>30</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1205,19 +1236,19 @@
         <v>1</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="D24" s="1">
-        <v>44978</v>
+        <v>45009</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G24" s="8">
-        <v>60</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1225,64 +1256,60 @@
         <v>1</v>
       </c>
       <c r="B25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" s="1">
+        <v>45009</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G25" s="8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="1">
-        <v>44978</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G25" s="8">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="9">
-        <v>1</v>
-      </c>
-      <c r="B26" s="9">
-        <v>2</v>
-      </c>
-      <c r="C26" s="10" t="s">
+      <c r="D26" s="1">
+        <v>45010</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G26" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D26" s="11">
-        <v>44979</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F26" s="10"/>
-      <c r="G26" s="12">
-        <v>60</v>
-      </c>
-      <c r="H26" s="9"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="9">
-        <v>1</v>
-      </c>
-      <c r="B27" s="9">
-        <v>2</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D27" s="11">
-        <v>44979</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F27" s="10"/>
-      <c r="G27" s="12">
-        <v>60</v>
-      </c>
-      <c r="H27" s="9"/>
+      <c r="D27" s="1">
+        <v>45010</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G27" s="8">
+        <v>60</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
@@ -1292,19 +1319,16 @@
         <v>3</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D28" s="1">
-        <v>45009</v>
+        <v>45010</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G28" s="8">
-        <v>10</v>
-      </c>
-      <c r="H28" t="s">
-        <v>49</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1315,16 +1339,16 @@
         <v>3</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="D29" s="1">
-        <v>45009</v>
+        <v>45010</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G29" s="8">
-        <v>60</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1335,17 +1359,20 @@
         <v>3</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="D30" s="1">
-        <v>45010</v>
+        <v>45011</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G30" s="8">
         <v>20</v>
       </c>
+      <c r="H30" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
@@ -1355,16 +1382,19 @@
         <v>3</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="D31" s="1">
-        <v>45010</v>
+        <v>45011</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G31" s="8">
-        <v>60</v>
+        <v>20</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1375,17 +1405,18 @@
         <v>3</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="D32" s="1">
-        <v>45010</v>
+        <v>45011</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G32" s="8">
-        <v>5</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="H32" s="3"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
@@ -1395,20 +1426,18 @@
         <v>3</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="D33" s="1">
-        <v>45011</v>
+        <v>45013</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G33" s="8">
-        <v>20</v>
-      </c>
-      <c r="H33" t="s">
-        <v>22</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="H33" s="3"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
@@ -1418,20 +1447,18 @@
         <v>3</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="D34" s="1">
         <v>45011</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G34" s="8">
         <v>20</v>
       </c>
-      <c r="H34" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="H34" s="3"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
@@ -1444,121 +1471,122 @@
         <v>43</v>
       </c>
       <c r="D35" s="1">
-        <v>45011</v>
+        <v>45013</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G35" s="8">
-        <v>20</v>
-      </c>
-      <c r="H35" s="3"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>1</v>
-      </c>
-      <c r="B36">
+      <c r="A36" s="9">
+        <v>1</v>
+      </c>
+      <c r="B36" s="9">
         <v>3</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D36" s="1">
-        <v>45013</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G36" s="8">
-        <v>60</v>
-      </c>
-      <c r="H36" s="3"/>
+      <c r="C36" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D36" s="11">
+        <v>44986</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F36" s="10"/>
+      <c r="G36" s="12">
+        <v>60</v>
+      </c>
+      <c r="H36" s="9"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>1</v>
-      </c>
-      <c r="B37">
+      <c r="A37" s="9">
+        <v>1</v>
+      </c>
+      <c r="B37" s="9">
         <v>3</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D37" s="1">
-        <v>45011</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G37" s="8">
-        <v>20</v>
-      </c>
-      <c r="H37" s="3"/>
+      <c r="C37" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37" s="11">
+        <v>44986</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F37" s="10"/>
+      <c r="G37" s="12">
+        <v>30</v>
+      </c>
+      <c r="H37" s="9"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1</v>
       </c>
       <c r="B38">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="D38" s="1">
-        <v>45013</v>
+        <v>44988</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G38" s="8">
-        <v>60</v>
+        <v>20</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="9">
-        <v>1</v>
-      </c>
-      <c r="B39" s="9">
-        <v>3</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D39" s="11">
-        <v>44986</v>
-      </c>
-      <c r="E39" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F39" s="10"/>
-      <c r="G39" s="12">
-        <v>60</v>
-      </c>
-      <c r="H39" s="9"/>
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D39" s="1">
+        <v>44989</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G39" s="8">
+        <v>20</v>
+      </c>
+      <c r="H39" s="3"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="9">
-        <v>1</v>
-      </c>
-      <c r="B40" s="9">
-        <v>3</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D40" s="11">
-        <v>44986</v>
-      </c>
-      <c r="E40" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F40" s="10"/>
-      <c r="G40" s="12">
-        <v>30</v>
-      </c>
-      <c r="H40" s="9"/>
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40">
+        <v>4</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" s="1">
+        <v>44990</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G40" s="8">
+        <v>60</v>
+      </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
@@ -1568,19 +1596,16 @@
         <v>4</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="D41" s="1">
-        <v>44988</v>
+        <v>44990</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G41" s="8">
-        <v>20</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -1591,155 +1616,94 @@
         <v>4</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="D42" s="1">
-        <v>44989</v>
+        <v>44993</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G42" s="8">
         <v>20</v>
       </c>
-      <c r="H42" s="3"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1</v>
       </c>
       <c r="B43">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D43" s="1">
-        <v>44990</v>
+        <v>44999</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G43" s="8">
-        <v>60</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>1</v>
-      </c>
-      <c r="B44">
-        <v>4</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D44" s="1">
-        <v>44990</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G44" s="8">
-        <v>60</v>
-      </c>
+      <c r="A44" s="9">
+        <v>1</v>
+      </c>
+      <c r="B44" s="9">
+        <v>5</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D44" s="11">
+        <v>44999</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F44" s="10"/>
+      <c r="G44" s="12">
+        <v>60</v>
+      </c>
+      <c r="H44" s="9"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>1</v>
-      </c>
-      <c r="B45">
-        <v>4</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D45" s="1">
-        <v>44993</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G45" s="8">
-        <v>20</v>
-      </c>
+      <c r="A45" s="17">
+        <v>1</v>
+      </c>
+      <c r="B45" s="17">
+        <v>5</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D45" s="19">
+        <v>45000</v>
+      </c>
+      <c r="E45" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="F45" s="18"/>
+      <c r="G45" s="20">
+        <v>0</v>
+      </c>
+      <c r="H45" s="17"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>1</v>
-      </c>
-      <c r="B46">
-        <v>5</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D46" s="1">
-        <v>44999</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G46" s="8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="9">
-        <v>1</v>
-      </c>
-      <c r="B47" s="9">
-        <v>5</v>
-      </c>
-      <c r="C47" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D47" s="11">
-        <v>44999</v>
-      </c>
-      <c r="E47" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F47" s="10"/>
-      <c r="G47" s="12">
-        <v>60</v>
-      </c>
-      <c r="H47" s="9"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="17">
-        <v>1</v>
-      </c>
-      <c r="B48" s="17">
-        <v>5</v>
-      </c>
-      <c r="C48" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D48" s="19">
-        <v>45000</v>
-      </c>
-      <c r="E48" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="20">
-        <v>0</v>
-      </c>
-      <c r="H48" s="17"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="21"/>
-      <c r="B49" s="21"/>
-      <c r="C49" s="22"/>
-      <c r="D49" s="23"/>
-      <c r="E49" s="23"/>
-      <c r="F49" s="22"/>
-      <c r="G49" s="24">
+      <c r="A46" s="21"/>
+      <c r="B46" s="21"/>
+      <c r="C46" s="22"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="23"/>
+      <c r="F46" s="22"/>
+      <c r="G46" s="24" t="e">
         <f>SUM([1]!Tabla3[Tiempo estimado (minutos)]) / 60</f>
-        <v>29.75</v>
-      </c>
-      <c r="H49" s="21"/>
+        <v>#REF!</v>
+      </c>
+      <c r="H46" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>